<commit_message>
finalized board, checked all errors
</commit_message>
<xml_diff>
--- a/gerberanddrillLower/BOM/RPD_Lower.xlsx
+++ b/gerberanddrillLower/BOM/RPD_Lower.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11004" windowHeight="9912" xr2:uid="{EFF542F9-6ABE-432F-AE4D-1D7EED908F97}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11004" windowHeight="9912" xr2:uid="{61DC7DB5-A83A-4609-82A0-C2A5FCAA40BD}"/>
   </bookViews>
   <sheets>
     <sheet name="RPD_Lower" sheetId="1" r:id="rId1"/>
@@ -746,7 +746,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C18B57BC-33BD-417D-AE97-95793A80338A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F33D6FF0-D2F3-4409-8DB9-12131C95AA19}">
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
added ams status and imd status and regenerated
</commit_message>
<xml_diff>
--- a/gerberanddrillLower/BOM/RPD_Lower.xlsx
+++ b/gerberanddrillLower/BOM/RPD_Lower.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11004" windowHeight="9912" xr2:uid="{61DC7DB5-A83A-4609-82A0-C2A5FCAA40BD}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11004" windowHeight="9912" xr2:uid="{57E21C80-D98F-43CA-8197-E81662DD025D}"/>
   </bookViews>
   <sheets>
     <sheet name="RPD_Lower" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="111">
   <si>
     <t>Comment</t>
   </si>
@@ -145,18 +145,6 @@
   </si>
   <si>
     <t>HDR1X10</t>
-  </si>
-  <si>
-    <t>Header 4</t>
-  </si>
-  <si>
-    <t>Header, 4-Pin</t>
-  </si>
-  <si>
-    <t>P5</t>
-  </si>
-  <si>
-    <t>HDR1X4</t>
   </si>
   <si>
     <t>MOSFET-P</t>
@@ -746,8 +734,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F33D6FF0-D2F3-4409-8DB9-12131C95AA19}">
-  <dimension ref="A1:F35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FF43268-F991-4006-A73A-155240781111}">
+  <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -993,7 +981,7 @@
         <v>42</v>
       </c>
       <c r="F12" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -1013,47 +1001,47 @@
         <v>46</v>
       </c>
       <c r="F13" s="3">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="D14" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="F14" s="3">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>46</v>
-      </c>
       <c r="F15" s="3">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -1061,56 +1049,56 @@
         <v>55</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F16" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F17" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F18" s="3">
         <v>2</v>
@@ -1118,19 +1106,19 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F19" s="3">
         <v>2</v>
@@ -1138,119 +1126,119 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F20" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="F21" s="3">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C22" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="E22" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F22" s="3">
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>74</v>
+        <v>9</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F23" s="3">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>58</v>
+        <v>11</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>9</v>
+        <v>72</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F24" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C25" s="2" t="s">
+      <c r="D25" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>76</v>
-      </c>
       <c r="E25" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F25" s="3">
         <v>1</v>
@@ -1281,13 +1269,13 @@
         <v>82</v>
       </c>
       <c r="B27" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="D27" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>85</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>82</v>
@@ -1298,10 +1286,10 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>83</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>87</v>
@@ -1310,7 +1298,7 @@
         <v>88</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F28" s="3">
         <v>1</v>
@@ -1347,7 +1335,7 @@
         <v>95</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>93</v>
@@ -1358,19 +1346,19 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="D31" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D31" s="2" t="s">
-        <v>98</v>
-      </c>
       <c r="E31" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F31" s="3">
         <v>1</v>
@@ -1390,7 +1378,7 @@
         <v>103</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="F32" s="3">
         <v>1</v>
@@ -1398,61 +1386,41 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B33" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D33" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C33" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>107</v>
-      </c>
       <c r="E33" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="F33" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="D34" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="C34" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>109</v>
-      </c>
       <c r="E34" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F34" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="F35" s="3">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed hole clearance issue
</commit_message>
<xml_diff>
--- a/gerberanddrillLower/BOM/RPD_Lower.xlsx
+++ b/gerberanddrillLower/BOM/RPD_Lower.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11004" windowHeight="9912" xr2:uid="{57E21C80-D98F-43CA-8197-E81662DD025D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11004" windowHeight="9912" xr2:uid="{D9D86763-BB3F-4573-B96F-549CE86B34C5}"/>
   </bookViews>
   <sheets>
     <sheet name="RPD_Lower" sheetId="1" r:id="rId1"/>
@@ -734,7 +734,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FF43268-F991-4006-A73A-155240781111}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C8C78B5-004F-40EF-B3E6-367EE9B5A582}">
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>